<commit_message>
update spreadsheet to track data translation
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="4360" windowWidth="37400" windowHeight="23040" tabRatio="500"/>
+    <workbookView xWindow="4140" yWindow="4360" windowWidth="37400" windowHeight="23040" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
     <sheet name="ADA Codes" sheetId="2" r:id="rId2"/>
     <sheet name="Conditons" sheetId="3" r:id="rId3"/>
+    <sheet name="Translated Files" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="215">
   <si>
     <t>Procedure Type</t>
   </si>
@@ -518,6 +519,165 @@
   </si>
   <si>
     <t>D0180</t>
+  </si>
+  <si>
+    <t>NDPBRN Practice</t>
+  </si>
+  <si>
+    <t>Practice 1</t>
+  </si>
+  <si>
+    <t>Practice 2</t>
+  </si>
+  <si>
+    <t>Practice 3</t>
+  </si>
+  <si>
+    <t>Practice 4</t>
+  </si>
+  <si>
+    <t>Practice 5</t>
+  </si>
+  <si>
+    <t>Practice 6</t>
+  </si>
+  <si>
+    <t>Practice 7</t>
+  </si>
+  <si>
+    <t>Practice 8</t>
+  </si>
+  <si>
+    <t>Practice 9</t>
+  </si>
+  <si>
+    <t>Practice 10</t>
+  </si>
+  <si>
+    <t>Practice 11</t>
+  </si>
+  <si>
+    <t>Practice 12</t>
+  </si>
+  <si>
+    <t>Practice 13</t>
+  </si>
+  <si>
+    <t>Practice 14</t>
+  </si>
+  <si>
+    <t>Practice 15</t>
+  </si>
+  <si>
+    <t>Practice 16</t>
+  </si>
+  <si>
+    <t>Practice 17</t>
+  </si>
+  <si>
+    <t>Practice 18</t>
+  </si>
+  <si>
+    <t>Practice 19</t>
+  </si>
+  <si>
+    <t>Practice 20</t>
+  </si>
+  <si>
+    <t>Practice 21</t>
+  </si>
+  <si>
+    <t>Practice 22</t>
+  </si>
+  <si>
+    <t>Practice 23</t>
+  </si>
+  <si>
+    <t>Practice 24</t>
+  </si>
+  <si>
+    <t>Practice 25</t>
+  </si>
+  <si>
+    <t>Practice 26</t>
+  </si>
+  <si>
+    <t>Practice 27</t>
+  </si>
+  <si>
+    <t>Practice 28</t>
+  </si>
+  <si>
+    <t>Practice 29</t>
+  </si>
+  <si>
+    <t>Practice 30</t>
+  </si>
+  <si>
+    <t>Practice 31</t>
+  </si>
+  <si>
+    <t>Practice 32</t>
+  </si>
+  <si>
+    <t>Practice 33</t>
+  </si>
+  <si>
+    <t>Practice 34</t>
+  </si>
+  <si>
+    <t>Practice 35</t>
+  </si>
+  <si>
+    <t>Practice 36</t>
+  </si>
+  <si>
+    <t>Practice 37</t>
+  </si>
+  <si>
+    <t>Practice 38</t>
+  </si>
+  <si>
+    <t>Practice 39</t>
+  </si>
+  <si>
+    <t>Practice 40</t>
+  </si>
+  <si>
+    <t>Practice 41</t>
+  </si>
+  <si>
+    <t>Practice 42</t>
+  </si>
+  <si>
+    <t>Practice 43</t>
+  </si>
+  <si>
+    <t>Practice 44</t>
+  </si>
+  <si>
+    <t>Practice 45</t>
+  </si>
+  <si>
+    <t>Practice 46</t>
+  </si>
+  <si>
+    <t>Practice 47</t>
+  </si>
+  <si>
+    <t>Practice 48</t>
+  </si>
+  <si>
+    <t>Practice 49</t>
+  </si>
+  <si>
+    <t>Practice 50</t>
+  </si>
+  <si>
+    <t>Pattent.ttl</t>
+  </si>
+  <si>
+    <t>Provider.ttl</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -1831,4 +1991,291 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove axiom file for fixed partual dentures and update spelling error in other axiom files: NDBPRN -> NDPBRN
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="1000" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3320" yWindow="500" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="228">
   <si>
     <t>Procedure Type</t>
   </si>
@@ -714,6 +714,12 @@
   </si>
   <si>
     <t>validating</t>
+  </si>
+  <si>
+    <t>surgic_tooth_extraction.ttl</t>
+  </si>
+  <si>
+    <t>pontic.ttl</t>
   </si>
 </sst>
 </file>
@@ -1273,9 +1279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1289,7 +1295,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="38">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="36">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1390,12 +1396,18 @@
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="B10" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1447,7 +1459,7 @@
     <col min="13" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" ht="38">
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="36">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -2033,11 +2045,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2055,9 +2067,10 @@
     <col min="11" max="11" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="19">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
         <v>162</v>
       </c>
@@ -2097,8 +2110,14 @@
       <c r="M1" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -2138,8 +2157,14 @@
       <c r="M2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -2179,8 +2204,14 @@
       <c r="M3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" t="s">
+        <v>225</v>
+      </c>
+      <c r="O3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -2220,63 +2251,69 @@
       <c r="M4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" t="s">
+        <v>225</v>
+      </c>
+      <c r="O4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
add procedure for root removal, dental implants, removable denturs
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35840" yWindow="3620" windowWidth="33180" windowHeight="20460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -1534,7 +1534,7 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
add noble metal implant crown, and update tracking spreadsheet
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-40300" yWindow="280" windowWidth="30000" windowHeight="18580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="256">
   <si>
     <t>Procedure Type</t>
   </si>
@@ -411,10 +411,6 @@
     <t>D2720</t>
   </si>
   <si>
-    <t>Dental
- Implant</t>
-  </si>
-  <si>
     <t>Oral
 Evaluation</t>
   </si>
@@ -790,6 +786,29 @@
   </si>
   <si>
     <t>New ADA codes added after discussion with Thankam/Zasmin</t>
+  </si>
+  <si>
+    <t>Dental Implant
+ Bodies</t>
+  </si>
+  <si>
+    <t>Dental Implant
+ Abutments</t>
+  </si>
+  <si>
+    <t>Dental Implant
+ Crowns</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Root Extraction</t>
+  </si>
+  <si>
+    <t>Pulp 
+Capping</t>
+  </si>
+  <si>
+    <t>Pulp
+Regeneration</t>
   </si>
 </sst>
 </file>
@@ -870,7 +889,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -932,8 +951,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -970,8 +1007,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1002,6 +1045,15 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1032,6 +1084,15 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1531,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1542,20 +1603,21 @@
     <col min="1" max="1" width="10.5" style="6" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" style="6"/>
-    <col min="5" max="5" width="17" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.5" style="6" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="62.83203125" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="6"/>
+    <col min="5" max="7" width="17" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="21.5" style="6" customWidth="1"/>
+    <col min="17" max="17" width="13.5" style="6" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.83203125" style="6" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="36">
+    <row r="1" spans="1:19" s="9" customFormat="1" ht="36">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -1571,33 +1633,48 @@
       <c r="E1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" s="12"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="S1" s="12"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="6" t="s">
         <v>69</v>
       </c>
@@ -1611,37 +1688,52 @@
         <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>140</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>240</v>
+        <v>135</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>143</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="6" t="s">
         <v>70</v>
       </c>
@@ -1655,31 +1747,46 @@
         <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>134</v>
+        <v>127</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>241</v>
+        <v>136</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>144</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="6" t="s">
         <v>71</v>
       </c>
@@ -1693,31 +1800,36 @@
         <v>9</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>135</v>
+        <v>128</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>232</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>238</v>
+        <v>137</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>145</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="6" t="s">
         <v>72</v>
       </c>
@@ -1731,28 +1843,30 @@
         <v>124</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>239</v>
+        <v>138</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>146</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="6" t="s">
         <v>73</v>
       </c>
@@ -1766,19 +1880,18 @@
         <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>130</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="6" t="s">
         <v>74</v>
       </c>
@@ -1792,19 +1905,18 @@
         <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>131</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
         <v>75</v>
       </c>
@@ -1818,16 +1930,15 @@
         <v>12</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>132</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="6" t="s">
         <v>76</v>
       </c>
@@ -1841,16 +1952,15 @@
         <v>13</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>133</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="6" t="s">
         <v>84</v>
       </c>
@@ -1864,16 +1974,15 @@
         <v>14</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>134</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="6" t="s">
         <v>85</v>
       </c>
@@ -1889,14 +1998,13 @@
       <c r="E11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="M11" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="6" t="s">
         <v>86</v>
       </c>
@@ -1909,14 +2017,14 @@
       <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="M12" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="6" t="s">
         <v>87</v>
       </c>
@@ -1929,14 +2037,14 @@
       <c r="D13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="M13" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="6" t="s">
         <v>77</v>
       </c>
@@ -1949,14 +2057,14 @@
       <c r="D14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="M14" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="6" t="s">
         <v>78</v>
       </c>
@@ -1969,14 +2077,14 @@
       <c r="D15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="M15" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="6" t="s">
         <v>79</v>
       </c>
@@ -1989,11 +2097,11 @@
       <c r="D16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
         <v>80</v>
       </c>
@@ -2006,8 +2114,11 @@
       <c r="D17" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>81</v>
       </c>
@@ -2021,7 +2132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:8">
       <c r="A19" s="6" t="s">
         <v>82</v>
       </c>
@@ -2035,7 +2146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>83</v>
       </c>
@@ -2043,62 +2154,62 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:8">
       <c r="D21" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:8">
       <c r="D22" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:8">
       <c r="D23" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:8">
       <c r="D24" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:8">
       <c r="D25" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:8">
       <c r="D26" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:8">
       <c r="D27" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:8">
       <c r="D28" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:8">
       <c r="D29" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:8">
       <c r="D30" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:8">
       <c r="D31" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:8">
       <c r="D32" s="6" t="s">
         <v>36</v>
       </c>
@@ -2239,425 +2350,425 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="N1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding new reasoned NDPBRN.owl to dental implant classes
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40300" yWindow="280" windowWidth="30000" windowHeight="18580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
working on (I think it is complete) the axioms for dental implant abutments
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9380" yWindow="1700" windowWidth="34760" windowHeight="20760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updating on axioms for procedures
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9380" yWindow="1700" windowWidth="34760" windowHeight="20760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7060" yWindow="1040" windowWidth="42400" windowHeight="22660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="262">
   <si>
     <t>Procedure Type</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Root Amputation</t>
-  </si>
-  <si>
-    <t>Dental Implant</t>
   </si>
   <si>
     <t>D2390</t>
@@ -809,6 +806,27 @@
   <si>
     <t>Pulp
 Regeneration</t>
+  </si>
+  <si>
+    <t>Root extaction</t>
+  </si>
+  <si>
+    <t>Dental Implant Body</t>
+  </si>
+  <si>
+    <t>Dental Implant Abutment</t>
+  </si>
+  <si>
+    <t>Dental Implant Crown</t>
+  </si>
+  <si>
+    <t>Pulp Cappping</t>
+  </si>
+  <si>
+    <t>Pulp Regeneration</t>
+  </si>
+  <si>
+    <t>Apicoectomy</t>
   </si>
 </sst>
 </file>
@@ -889,8 +907,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1014,7 +1036,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1054,6 +1076,8 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1093,6 +1117,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1427,11 +1453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1450,16 +1476,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1467,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1477,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1487,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1497,27 +1523,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>261</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1526,58 +1552,113 @@
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>255</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>259</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>260</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>46</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1594,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1631,471 +1712,471 @@
         <v>4</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="N1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>252</v>
-      </c>
       <c r="Q1" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S1" s="12"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>245</v>
+        <v>142</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>244</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S2" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>246</v>
+        <v>143</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>245</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>241</v>
+        <v>144</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>240</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>242</v>
+        <v>145</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>241</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>243</v>
+        <v>146</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>242</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>244</v>
+        <v>147</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>243</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="M12" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="M13" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="M14" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="M15" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -2103,16 +2184,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -2120,148 +2201,148 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="D21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="D22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="D23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="D24" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="D25" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="D26" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="D27" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="D28" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="D29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="D30" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="D31" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="D32" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="4:4">
       <c r="D39" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="4:4">
       <c r="D40" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="4:4">
       <c r="D41" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="4:4">
       <c r="D42" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2292,23 +2373,23 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2350,425 +2431,425 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="N1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add first pass for axiom template for existing services
</commit_message>
<xml_diff>
--- a/src/data/NDPBRN data translation tracking.xlsx
+++ b/src/data/NDPBRN data translation tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7900" yWindow="540" windowWidth="38120" windowHeight="21400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="262">
   <si>
     <t>Procedure Type</t>
   </si>
@@ -824,6 +824,9 @@
   </si>
   <si>
     <t>Apicoectomy</t>
+  </si>
+  <si>
+    <t>finsihed</t>
   </si>
 </sst>
 </file>
@@ -881,18 +884,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -989,7 +986,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1016,9 +1013,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1452,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1579,6 +1573,9 @@
       <c r="A11" s="3" t="s">
         <v>259</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>261</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
@@ -1687,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1744,7 +1741,7 @@
       <c r="K1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>251</v>
       </c>
       <c r="M1" s="5" t="s">
@@ -1765,7 +1762,7 @@
       <c r="R1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="S1" s="12"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="6" t="s">
@@ -1783,10 +1780,10 @@
       <c r="E2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>229</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -1801,28 +1798,28 @@
       <c r="K2" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>232</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="12" t="s">
         <v>234</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="S2" s="15"/>
+      <c r="S2" s="14"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="6" t="s">
@@ -1840,10 +1837,10 @@
       <c r="E3" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="12" t="s">
         <v>230</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -1855,22 +1852,22 @@
       <c r="K3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>233</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="12" t="s">
         <v>235</v>
       </c>
       <c r="R3" s="6" t="s">
@@ -1893,7 +1890,7 @@
       <c r="E4" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="12" t="s">
         <v>231</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -1908,12 +1905,12 @@
       <c r="M4" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13" t="s">
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12" t="s">
         <v>236</v>
       </c>
       <c r="R4" s="6" t="s">
@@ -1945,12 +1942,12 @@
       <c r="M5" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13" t="s">
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12" t="s">
         <v>237</v>
       </c>
       <c r="R5" s="6" t="s">
@@ -1976,11 +1973,11 @@
       <c r="M6" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="N6" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="6" t="s">
@@ -2001,11 +1998,11 @@
       <c r="M7" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N7" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
@@ -2026,8 +2023,8 @@
       <c r="M8" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6" t="s">
@@ -2048,8 +2045,8 @@
       <c r="M9" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6" t="s">
@@ -2070,8 +2067,8 @@
       <c r="M10" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="6" t="s">
@@ -2092,8 +2089,8 @@
       <c r="M11" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="6" t="s">
@@ -2108,9 +2105,9 @@
       <c r="D12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="M12" s="6" t="s">
         <v>152</v>
       </c>
@@ -2128,9 +2125,9 @@
       <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="M13" s="6" t="s">
         <v>153</v>
       </c>
@@ -2148,9 +2145,9 @@
       <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="M14" s="6" t="s">
         <v>154</v>
       </c>
@@ -2168,9 +2165,9 @@
       <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
       <c r="M15" s="6" t="s">
         <v>155</v>
       </c>
@@ -2188,9 +2185,9 @@
       <c r="D16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
@@ -2205,9 +2202,9 @@
       <c r="D17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">

</xml_diff>